<commit_message>
updated ksom wallfollow analysis
</commit_message>
<xml_diff>
--- a/results_analysis/ksom_wallFollow_01_hold_01.xlsx
+++ b/results_analysis/ksom_wallFollow_01_hold_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab_fp\results_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75064BE4-1F64-4024-ACEB-314F689C4210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1290A7CA-CB7F-41B3-9A98-D02DEEE71AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{FE0D8406-1939-42F0-B5EC-F1A66084C35D}"/>
   </bookViews>
   <sheets>
     <sheet name="hp_best" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="28">
   <si>
     <t>Algorithm</t>
   </si>
@@ -106,6 +106,27 @@
   <si>
     <t>HPO = Best</t>
   </si>
+  <si>
+    <t>Comparison: HPO=Best - HPO=1</t>
+  </si>
+  <si>
+    <t>Comparison: KSOM-EF - KSOM-GD</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>Comparison: Labeling Strategies, HPO = 1</t>
+  </si>
+  <si>
+    <t>Comparison: Labeling Strategies, HPO = best</t>
+  </si>
+  <si>
+    <t>HPO=1</t>
+  </si>
+  <si>
+    <t>HPO=Best</t>
+  </si>
 </sst>
 </file>
 
@@ -115,8 +136,16 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -132,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -445,11 +474,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -559,6 +750,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -571,16 +772,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,49 +1166,49 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="39" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="40"/>
-      <c r="N2" s="39" t="s">
+      <c r="M2" s="44"/>
+      <c r="N2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="41"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="45"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1255,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1302,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -1100,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -1135,7 +1382,7 @@
       <c r="L6" s="31">
         <v>3.90625E-3</v>
       </c>
-      <c r="M6" s="43">
+      <c r="M6" s="39">
         <v>0.5</v>
       </c>
       <c r="N6" s="20">
@@ -1145,7 +1392,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -1182,7 +1429,7 @@
       <c r="L7" s="31">
         <v>0.125</v>
       </c>
-      <c r="M7" s="43">
+      <c r="M7" s="39">
         <v>-0.25</v>
       </c>
       <c r="N7" s="20">
@@ -1192,7 +1439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -1230,19 +1477,19 @@
       <c r="M8" s="20">
         <v>-0.5</v>
       </c>
-      <c r="N8" s="45">
+      <c r="N8" s="41">
         <v>16</v>
       </c>
       <c r="O8" s="21">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="44">
+      <c r="C9" s="40">
         <v>256</v>
       </c>
       <c r="D9" s="22">
@@ -1282,29 +1529,29 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="46"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C12" s="46"/>
-      <c r="L12" s="46"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="L13" s="46"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="46"/>
-      <c r="E14" s="46"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E15" s="46"/>
-      <c r="L15" s="46"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="E16" s="46"/>
-      <c r="L16" s="46"/>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C11" s="42"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C12" s="42"/>
+      <c r="L12" s="42"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C14" s="42"/>
+      <c r="E14" s="42"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E15" s="42"/>
+      <c r="L15" s="42"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="E16" s="42"/>
+      <c r="L16" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1325,32 +1572,32 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1414,7 +1661,7 @@
         <v>0.81551618814905302</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -1444,7 +1691,7 @@
         <v>0.92058643860720801</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -1474,7 +1721,7 @@
         <v>0.81185094685400105</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1506,7 +1753,7 @@
         <v>0.91569945021380605</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -1536,7 +1783,7 @@
         <v>0.79352474037874199</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -1566,22 +1813,22 @@
         <v>0.78313989004276097</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -1613,7 +1860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
@@ -1645,7 +1892,7 @@
         <v>0.80452046426389701</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -1675,7 +1922,7 @@
         <v>0.92852779474648806</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -1705,7 +1952,7 @@
         <v>0.81246182040317705</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>2</v>
       </c>
@@ -1737,7 +1984,7 @@
         <v>0.91936469150885802</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -1767,7 +2014,7 @@
         <v>0.74587660354306695</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -1808,35 +2055,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C2E4AB-28B4-4560-9CA9-8AF5549FD7E4}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.33203125" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+      <c r="L2" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="45"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -1867,8 +2129,38 @@
       <c r="J3" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="R3" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>1</v>
       </c>
@@ -1881,10 +2173,10 @@
       <c r="D4" s="24">
         <v>0.75729993891264502</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="47">
         <v>0.75968234575442894</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="47">
         <v>0.78894318875992697</v>
       </c>
       <c r="G4" s="24">
@@ -1893,14 +2185,52 @@
       <c r="H4" s="24">
         <v>0.74654856444716</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="47">
         <v>0.772327428222358</v>
       </c>
       <c r="J4" s="25">
         <v>0.75778863775198502</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="61">
+        <f>C4-C7</f>
+        <v>-7.8191814294440443E-3</v>
+      </c>
+      <c r="O4" s="61">
+        <f t="shared" ref="O4:U4" si="0">D4-D7</f>
+        <v>-6.5974343310939432E-3</v>
+      </c>
+      <c r="P4" s="61">
+        <f t="shared" si="0"/>
+        <v>-1.0262675626145024E-2</v>
+      </c>
+      <c r="Q4" s="61">
+        <f t="shared" si="0"/>
+        <v>-0.11912034208918698</v>
+      </c>
+      <c r="R4" s="61">
+        <f t="shared" si="0"/>
+        <v>-0.14465485644471598</v>
+      </c>
+      <c r="S4" s="61">
+        <f t="shared" si="0"/>
+        <v>-0.14893097128894295</v>
+      </c>
+      <c r="T4" s="61">
+        <f t="shared" si="0"/>
+        <v>-0.12718387293830202</v>
+      </c>
+      <c r="U4" s="63">
+        <f t="shared" si="0"/>
+        <v>-0.14648747709224197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="36"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -1908,16 +2238,16 @@
       <c r="C5" s="26">
         <v>0.87373243738546102</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="48">
         <v>0.89499083689676195</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="48">
         <v>0.90213805742211395</v>
       </c>
       <c r="F5" s="26">
         <v>0.88961514966402</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="48">
         <v>0.90091631032376296</v>
       </c>
       <c r="H5" s="26">
@@ -1929,8 +2259,44 @@
       <c r="J5" s="27">
         <v>0.89022602321319499</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="7"/>
+      <c r="M5" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="N5" s="61">
+        <f t="shared" ref="N5:N6" si="1">C5-C8</f>
+        <v>0.36994502138057406</v>
+      </c>
+      <c r="O5" s="61">
+        <f t="shared" ref="O5:U5" si="2">D5-D8</f>
+        <v>0.14667073915699391</v>
+      </c>
+      <c r="P5" s="61">
+        <f t="shared" si="2"/>
+        <v>0.168845448992059</v>
+      </c>
+      <c r="Q5" s="61">
+        <f t="shared" si="2"/>
+        <v>0.11093463653023905</v>
+      </c>
+      <c r="R5" s="61">
+        <f t="shared" si="2"/>
+        <v>0.16811240073304801</v>
+      </c>
+      <c r="S5" s="61">
+        <f t="shared" si="2"/>
+        <v>-1.0507025045816021E-2</v>
+      </c>
+      <c r="T5" s="61">
+        <f t="shared" si="2"/>
+        <v>0.18472816127061698</v>
+      </c>
+      <c r="U5" s="63">
+        <f t="shared" si="2"/>
+        <v>0.11649358582773395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="36"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -1944,23 +2310,59 @@
       <c r="E6" s="26">
         <v>0.74263897373243803</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="48">
         <v>0.79456322541234004</v>
       </c>
       <c r="G6" s="26">
         <v>0.76304215027489297</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="48">
         <v>0.76102626756261504</v>
       </c>
       <c r="I6" s="26">
         <v>0.73824068417837496</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="49">
         <v>0.77067806963958496</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L6" s="7"/>
+      <c r="M6" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="61">
+        <f t="shared" si="1"/>
+        <v>-9.6456933414783008E-2</v>
+      </c>
+      <c r="O6" s="61">
+        <f t="shared" ref="O6:U6" si="3">D6-D9</f>
+        <v>-1.9547953573609833E-3</v>
+      </c>
+      <c r="P6" s="61">
+        <f t="shared" si="3"/>
+        <v>-1.832620647519434E-4</v>
+      </c>
+      <c r="Q6" s="61">
+        <f t="shared" si="3"/>
+        <v>9.7739767868099126E-4</v>
+      </c>
+      <c r="R6" s="61">
+        <f t="shared" si="3"/>
+        <v>1.649358582773397E-2</v>
+      </c>
+      <c r="S6" s="61">
+        <f t="shared" si="3"/>
+        <v>2.7061698228467046E-2</v>
+      </c>
+      <c r="T6" s="61">
+        <f t="shared" si="3"/>
+        <v>-3.359804520464027E-3</v>
+      </c>
+      <c r="U6" s="63">
+        <f t="shared" si="3"/>
+        <v>3.2254123396456946E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
         <v>2</v>
       </c>
@@ -1976,10 +2378,10 @@
       <c r="E7" s="26">
         <v>0.76994502138057397</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="48">
         <v>0.90806353084911395</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="48">
         <v>0.90128283445326796</v>
       </c>
       <c r="H7" s="26">
@@ -1988,11 +2390,49 @@
       <c r="I7" s="26">
         <v>0.89951130116066003</v>
       </c>
-      <c r="J7" s="27">
+      <c r="J7" s="49">
         <v>0.90427611484422699</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="62">
+        <f>C13-C16</f>
+        <v>3.9706780696402433E-4</v>
+      </c>
+      <c r="O7" s="62">
+        <f t="shared" ref="O7:U7" si="4">D13-D16</f>
+        <v>8.4196701282833963E-2</v>
+      </c>
+      <c r="P7" s="62">
+        <f t="shared" si="4"/>
+        <v>9.170433720219906E-2</v>
+      </c>
+      <c r="Q7" s="62">
+        <f t="shared" si="4"/>
+        <v>-0.10222357971899798</v>
+      </c>
+      <c r="R7" s="62">
+        <f t="shared" si="4"/>
+        <v>-0.12988393402565701</v>
+      </c>
+      <c r="S7" s="62">
+        <f t="shared" si="4"/>
+        <v>-0.12786194257788597</v>
+      </c>
+      <c r="T7" s="62">
+        <f t="shared" si="4"/>
+        <v>-0.10283445326817398</v>
+      </c>
+      <c r="U7" s="64">
+        <f t="shared" si="4"/>
+        <v>-0.13229077580940696</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="36"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -2006,23 +2446,59 @@
       <c r="E8" s="26">
         <v>0.73329260843005495</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="48">
         <v>0.77868051313378095</v>
       </c>
       <c r="G8" s="26">
         <v>0.73280390959071495</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="48">
         <v>0.75137446548564502</v>
       </c>
       <c r="I8" s="26">
         <v>0.70861331704337205</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="49">
         <v>0.77373243738546105</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="7"/>
+      <c r="M8" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="N8" s="62">
+        <f t="shared" ref="N8:N9" si="5">C14-C17</f>
+        <v>0.37040317654245603</v>
+      </c>
+      <c r="O8" s="62">
+        <f t="shared" ref="O8:U8" si="6">D14-D17</f>
+        <v>0.43002443494196702</v>
+      </c>
+      <c r="P8" s="62">
+        <f t="shared" si="6"/>
+        <v>0.42511912034208904</v>
+      </c>
+      <c r="Q8" s="62">
+        <f t="shared" si="6"/>
+        <v>0.40000610873549203</v>
+      </c>
+      <c r="R8" s="62">
+        <f t="shared" si="6"/>
+        <v>0.42336591325595596</v>
+      </c>
+      <c r="S8" s="62">
+        <f t="shared" si="6"/>
+        <v>0.26657910812461799</v>
+      </c>
+      <c r="T8" s="62">
+        <f t="shared" si="6"/>
+        <v>0.40842394624312806</v>
+      </c>
+      <c r="U8" s="64">
+        <f t="shared" si="6"/>
+        <v>0.41855833842394702</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="37"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -2030,16 +2506,16 @@
       <c r="C9" s="28">
         <v>0.67672571777641999</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="50">
         <v>0.75442883323152099</v>
       </c>
       <c r="E9" s="28">
         <v>0.74282223579718998</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="50">
         <v>0.79358582773365904</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G9" s="50">
         <v>0.746548564447159</v>
       </c>
       <c r="H9" s="28">
@@ -2051,23 +2527,71 @@
       <c r="J9" s="29">
         <v>0.73842394624312802</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+      <c r="L9" s="8"/>
+      <c r="M9" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="65">
+        <f t="shared" si="5"/>
+        <v>-2.1429444105070972E-2</v>
+      </c>
+      <c r="O9" s="65">
+        <f t="shared" ref="O9:U9" si="7">D15-D18</f>
+        <v>0.13357971899816701</v>
+      </c>
+      <c r="P9" s="65">
+        <f t="shared" si="7"/>
+        <v>0.12293830177153298</v>
+      </c>
+      <c r="Q9" s="65">
+        <f t="shared" si="7"/>
+        <v>0.14503359804520499</v>
+      </c>
+      <c r="R9" s="65">
+        <f t="shared" si="7"/>
+        <v>7.8442272449603001E-2</v>
+      </c>
+      <c r="S9" s="65">
+        <f t="shared" si="7"/>
+        <v>0.10725106902871107</v>
+      </c>
+      <c r="T9" s="65">
+        <f t="shared" si="7"/>
+        <v>9.1392791692120001E-2</v>
+      </c>
+      <c r="U9" s="66">
+        <f t="shared" si="7"/>
+        <v>0.12151496640195503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+      <c r="L11" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="44"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="44"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="44"/>
+      <c r="T11" s="44"/>
+      <c r="U11" s="45"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -2098,8 +2622,38 @@
       <c r="J12" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -2112,10 +2666,10 @@
       <c r="D13" s="24">
         <v>0.78078191814294395</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="47">
         <v>0.78249847281612706</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="47">
         <v>0.79218692730604801</v>
       </c>
       <c r="G13" s="24">
@@ -2124,14 +2678,52 @@
       <c r="H13" s="24">
         <v>0.76584605986560805</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="47">
         <v>0.79124007330482604</v>
       </c>
       <c r="J13" s="25">
         <v>0.762083078802688</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L13" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="57">
+        <f t="shared" ref="N13" si="8">C4-MAX(C4:C6)</f>
+        <v>-0.18576664630421502</v>
+      </c>
+      <c r="O13" s="57">
+        <f t="shared" ref="O13" si="9">D4-MAX(D4:D6)</f>
+        <v>-0.13769089798411693</v>
+      </c>
+      <c r="P13" s="57">
+        <f t="shared" ref="P13" si="10">E4-MAX(E4:E6)</f>
+        <v>-0.142455711667685</v>
+      </c>
+      <c r="Q13" s="57">
+        <f t="shared" ref="Q13" si="11">F4-MAX(F4:F6)</f>
+        <v>-0.10067196090409303</v>
+      </c>
+      <c r="R13" s="57">
+        <f t="shared" ref="R13" si="12">G4-MAX(G4:G6)</f>
+        <v>-0.14428833231521099</v>
+      </c>
+      <c r="S13" s="57">
+        <f t="shared" ref="S13" si="13">H4-MAX(H4:H6)</f>
+        <v>-1.4477703115455043E-2</v>
+      </c>
+      <c r="T13" s="57">
+        <f t="shared" ref="T13" si="14">I4-MAX(I4:I6)</f>
+        <v>-0.12101405009163102</v>
+      </c>
+      <c r="U13" s="58">
+        <f t="shared" ref="U13" si="15">J4-MAX(J4:J6)</f>
+        <v>-0.13243738546120998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -2139,7 +2731,7 @@
       <c r="C14" s="26">
         <v>0.860384850335981</v>
       </c>
-      <c r="D14" s="26">
+      <c r="D14" s="48">
         <v>0.89926084300549802</v>
       </c>
       <c r="E14" s="26">
@@ -2148,7 +2740,7 @@
       <c r="F14" s="26">
         <v>0.89678680513133802</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="48">
         <v>0.90042150274893096</v>
       </c>
       <c r="H14" s="26">
@@ -2157,11 +2749,47 @@
       <c r="I14" s="26">
         <v>0.88067196090409305</v>
       </c>
-      <c r="J14" s="27">
+      <c r="J14" s="49">
         <v>0.89924862553451501</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="7"/>
+      <c r="M14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="67">
+        <f t="shared" ref="N14" si="16">C5-MAX(C4:C6)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="67">
+        <f t="shared" ref="O14" si="17">D5-MAX(D4:D6)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="67">
+        <f t="shared" ref="P14" si="18">E5-MAX(E4:E6)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="67">
+        <f t="shared" ref="Q14" si="19">F5-MAX(F4:F6)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="67">
+        <f t="shared" ref="R14" si="20">G5-MAX(G4:G6)</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="67">
+        <f t="shared" ref="S14" si="21">H5-MAX(H4:H6)</f>
+        <v>-2.0158827122786049E-2</v>
+      </c>
+      <c r="T14" s="67">
+        <f t="shared" ref="T14" si="22">I5-MAX(I4:I6)</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="69">
+        <f t="shared" ref="U14" si="23">J5-MAX(J4:J6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -2169,13 +2797,13 @@
       <c r="C15" s="26">
         <v>0.63578497251068999</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="48">
         <v>0.76373854612095304</v>
       </c>
-      <c r="E15" s="26">
+      <c r="E15" s="48">
         <v>0.77511301160659696</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="48">
         <v>0.78059865607819201</v>
       </c>
       <c r="G15" s="26">
@@ -2190,8 +2818,44 @@
       <c r="J15" s="27">
         <v>0.76282223579719</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L15" s="7"/>
+      <c r="M15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="67">
+        <f>C6-MAX(C4:C6)</f>
+        <v>-0.29346365302382404</v>
+      </c>
+      <c r="O15" s="67">
+        <f t="shared" ref="O15:U15" si="24">D6-MAX(D4:D6)</f>
+        <v>-0.14251679902260195</v>
+      </c>
+      <c r="P15" s="67">
+        <f t="shared" si="24"/>
+        <v>-0.15949908368967591</v>
+      </c>
+      <c r="Q15" s="67">
+        <f t="shared" si="24"/>
+        <v>-9.5051924251679965E-2</v>
+      </c>
+      <c r="R15" s="67">
+        <f t="shared" si="24"/>
+        <v>-0.13787416004886999</v>
+      </c>
+      <c r="S15" s="67">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="T15" s="67">
+        <f t="shared" si="24"/>
+        <v>-0.15510079413561406</v>
+      </c>
+      <c r="U15" s="69">
+        <f t="shared" si="24"/>
+        <v>-0.11954795357361003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -2207,28 +2871,66 @@
       <c r="E16" s="26">
         <v>0.690794135613928</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="48">
         <v>0.89441050702504599</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="48">
         <v>0.89552229688454499</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="48">
         <v>0.89370800244349402</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="48">
         <v>0.89407452657300002</v>
       </c>
-      <c r="J16" s="27">
+      <c r="J16" s="49">
         <v>0.89437385461209495</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L16" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" s="67">
+        <f>C7-MAX(C7:C9)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="67">
+        <f t="shared" ref="O16:U16" si="25">D7-MAX(D7:D9)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="67">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="67">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="R16" s="67">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="S16" s="67">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="T16" s="67">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="69">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="48">
         <v>0.48998167379352497</v>
       </c>
       <c r="D17" s="26">
@@ -2237,13 +2939,13 @@
       <c r="E17" s="26">
         <v>0.47143555284056199</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="48">
         <v>0.49678069639584599</v>
       </c>
       <c r="G17" s="26">
         <v>0.477055589492975</v>
       </c>
-      <c r="H17" s="26">
+      <c r="H17" s="48">
         <v>0.49490531459987802</v>
       </c>
       <c r="I17" s="26">
@@ -2252,19 +2954,55 @@
       <c r="J17" s="27">
         <v>0.48069028711056799</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="7"/>
+      <c r="M17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="67">
+        <f>C8-MAX(C7:C9)</f>
+        <v>-0.19199755650580308</v>
+      </c>
+      <c r="O17" s="67">
+        <f t="shared" ref="O17:U17" si="26">D8-MAX(D7:D9)</f>
+        <v>-1.5577275503970922E-2</v>
+      </c>
+      <c r="P17" s="67">
+        <f t="shared" si="26"/>
+        <v>-3.665241295051902E-2</v>
+      </c>
+      <c r="Q17" s="67">
+        <f t="shared" si="26"/>
+        <v>-0.129383017715333</v>
+      </c>
+      <c r="R17" s="67">
+        <f t="shared" si="26"/>
+        <v>-0.168478924862553</v>
+      </c>
+      <c r="S17" s="67">
+        <f t="shared" si="26"/>
+        <v>-0.14410507025045793</v>
+      </c>
+      <c r="T17" s="67">
+        <f t="shared" si="26"/>
+        <v>-0.19089798411728798</v>
+      </c>
+      <c r="U17" s="69">
+        <f t="shared" si="26"/>
+        <v>-0.13054367745876594</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="38"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="50">
         <v>0.65721441661576097</v>
       </c>
       <c r="D18" s="28">
         <v>0.63015882712278604</v>
       </c>
-      <c r="E18" s="28">
+      <c r="E18" s="50">
         <v>0.65217470983506398</v>
       </c>
       <c r="F18" s="28">
@@ -2273,7 +3011,7 @@
       <c r="G18" s="28">
         <v>0.64293830177153299</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="50">
         <v>0.65610873549175297</v>
       </c>
       <c r="I18" s="28">
@@ -2282,13 +3020,595 @@
       <c r="J18" s="29">
         <v>0.64130726939523497</v>
       </c>
+      <c r="L18" s="8"/>
+      <c r="M18" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N18" s="68">
+        <f>C9-MAX(C7:C9)</f>
+        <v>-1.9059254734270059E-2</v>
+      </c>
+      <c r="O18" s="68">
+        <f t="shared" ref="O18:U18" si="27">D9-MAX(D7:D9)</f>
+        <v>-9.4685400122179741E-3</v>
+      </c>
+      <c r="P18" s="68">
+        <f t="shared" si="27"/>
+        <v>-2.712278558338399E-2</v>
+      </c>
+      <c r="Q18" s="68">
+        <f t="shared" si="27"/>
+        <v>-0.11447770311545491</v>
+      </c>
+      <c r="R18" s="68">
+        <f t="shared" si="27"/>
+        <v>-0.15473427000610895</v>
+      </c>
+      <c r="S18" s="68">
+        <f t="shared" si="27"/>
+        <v>-0.16151496640195495</v>
+      </c>
+      <c r="T18" s="68">
+        <f t="shared" si="27"/>
+        <v>-0.15791081246182104</v>
+      </c>
+      <c r="U18" s="70">
+        <f t="shared" si="27"/>
+        <v>-0.16585216860109897</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="45"/>
+      <c r="L20" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="44"/>
+      <c r="N20" s="44"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="44"/>
+      <c r="R20" s="44"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="44"/>
+      <c r="U20" s="45"/>
+    </row>
+    <row r="21" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="57">
+        <f>C13-C4</f>
+        <v>7.0494807574830176E-3</v>
+      </c>
+      <c r="D22" s="57">
+        <f t="shared" ref="D22:J22" si="28">D13-D4</f>
+        <v>2.3481979230298933E-2</v>
+      </c>
+      <c r="E22" s="57">
+        <f t="shared" si="28"/>
+        <v>2.281612706169811E-2</v>
+      </c>
+      <c r="F22" s="57">
+        <f t="shared" si="28"/>
+        <v>3.2437385461210333E-3</v>
+      </c>
+      <c r="G22" s="57">
+        <f t="shared" si="28"/>
+        <v>9.0103848503360062E-3</v>
+      </c>
+      <c r="H22" s="57">
+        <f t="shared" si="28"/>
+        <v>1.9297495418448052E-2</v>
+      </c>
+      <c r="I22" s="57">
+        <f t="shared" si="28"/>
+        <v>1.8912645082468038E-2</v>
+      </c>
+      <c r="J22" s="58">
+        <f t="shared" si="28"/>
+        <v>4.2944410507029795E-3</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="57">
+        <f>C13-MAX(C13:C15)</f>
+        <v>-0.16536957849725198</v>
+      </c>
+      <c r="O22" s="57">
+        <f t="shared" ref="O22:U22" si="29">D13-MAX(D13:D15)</f>
+        <v>-0.11847892486255407</v>
+      </c>
+      <c r="P22" s="57">
+        <f t="shared" si="29"/>
+        <v>-0.11405620036652397</v>
+      </c>
+      <c r="Q22" s="57">
+        <f t="shared" si="29"/>
+        <v>-0.10459987782529001</v>
+      </c>
+      <c r="R22" s="57">
+        <f t="shared" si="29"/>
+        <v>-0.13478313989004298</v>
+      </c>
+      <c r="S22" s="57">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="T22" s="57">
+        <f t="shared" si="29"/>
+        <v>-8.9431887599267013E-2</v>
+      </c>
+      <c r="U22" s="58">
+        <f t="shared" si="29"/>
+        <v>-0.13716554673182701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7"/>
+      <c r="B23" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="57">
+        <f t="shared" ref="C23:J27" si="30">C14-C5</f>
+        <v>-1.3347587049480025E-2</v>
+      </c>
+      <c r="D23" s="57">
+        <f t="shared" si="30"/>
+        <v>4.2700061087360686E-3</v>
+      </c>
+      <c r="E23" s="57">
+        <f t="shared" si="30"/>
+        <v>-5.5833842394629185E-3</v>
+      </c>
+      <c r="F23" s="57">
+        <f t="shared" si="30"/>
+        <v>7.1716554673180166E-3</v>
+      </c>
+      <c r="G23" s="57">
+        <f t="shared" si="30"/>
+        <v>-4.9480757483200133E-4</v>
+      </c>
+      <c r="H23" s="57">
+        <f t="shared" si="30"/>
+        <v>2.0616982284667018E-2</v>
+      </c>
+      <c r="I23" s="57">
+        <f t="shared" si="30"/>
+        <v>-1.266951740989597E-2</v>
+      </c>
+      <c r="J23" s="58">
+        <f t="shared" si="30"/>
+        <v>9.0226023213200168E-3</v>
+      </c>
+      <c r="L23" s="7"/>
+      <c r="M23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="67">
+        <f>C14-MAX(C13:C15)</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="67">
+        <f t="shared" ref="O23:U23" si="31">D14-MAX(D13:D15)</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="67">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="67">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="67">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="S23" s="67">
+        <f t="shared" si="31"/>
+        <v>-4.3616371411120403E-3</v>
+      </c>
+      <c r="T23" s="67">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="U23" s="69">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7"/>
+      <c r="B24" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="57">
+        <f t="shared" si="30"/>
+        <v>5.5516188149053014E-2</v>
+      </c>
+      <c r="D24" s="57">
+        <f t="shared" si="30"/>
+        <v>1.1264508246793037E-2</v>
+      </c>
+      <c r="E24" s="57">
+        <f t="shared" si="30"/>
+        <v>3.2474037874158923E-2</v>
+      </c>
+      <c r="F24" s="57">
+        <f t="shared" si="30"/>
+        <v>-1.3964569334148025E-2</v>
+      </c>
+      <c r="G24" s="57">
+        <f t="shared" si="30"/>
+        <v>-4.1661576053756977E-2</v>
+      </c>
+      <c r="H24" s="57">
+        <f t="shared" si="30"/>
+        <v>2.3335369578489917E-3</v>
+      </c>
+      <c r="I24" s="57">
+        <f t="shared" si="30"/>
+        <v>-1.445326817348791E-2</v>
+      </c>
+      <c r="J24" s="58">
+        <f t="shared" si="30"/>
+        <v>-7.8558338423949658E-3</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="67">
+        <f>C15-MAX(C13:C15)</f>
+        <v>-0.22459987782529101</v>
+      </c>
+      <c r="O24" s="67">
+        <f t="shared" ref="O24:U24" si="32">D15-MAX(D13:D15)</f>
+        <v>-0.13552229688454498</v>
+      </c>
+      <c r="P24" s="67">
+        <f t="shared" si="32"/>
+        <v>-0.12144166157605407</v>
+      </c>
+      <c r="Q24" s="67">
+        <f t="shared" si="32"/>
+        <v>-0.11618814905314601</v>
+      </c>
+      <c r="R24" s="67">
+        <f t="shared" si="32"/>
+        <v>-0.17904092852779496</v>
+      </c>
+      <c r="S24" s="67">
+        <f t="shared" si="32"/>
+        <v>-2.4862553451440172E-3</v>
+      </c>
+      <c r="T24" s="67">
+        <f t="shared" si="32"/>
+        <v>-0.156884544899206</v>
+      </c>
+      <c r="U24" s="69">
+        <f t="shared" si="32"/>
+        <v>-0.13642638973732502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="57">
+        <f t="shared" si="30"/>
+        <v>-1.166768478925051E-3</v>
+      </c>
+      <c r="D25" s="57">
+        <f t="shared" si="30"/>
+        <v>-6.7312156383628974E-2</v>
+      </c>
+      <c r="E25" s="57">
+        <f t="shared" si="30"/>
+        <v>-7.9150885766645973E-2</v>
+      </c>
+      <c r="F25" s="57">
+        <f t="shared" si="30"/>
+        <v>-1.3653023824067967E-2</v>
+      </c>
+      <c r="G25" s="57">
+        <f t="shared" si="30"/>
+        <v>-5.7605375687229676E-3</v>
+      </c>
+      <c r="H25" s="57">
+        <f t="shared" si="30"/>
+        <v>-1.7715332926089289E-3</v>
+      </c>
+      <c r="I25" s="57">
+        <f t="shared" si="30"/>
+        <v>-5.4367745876600093E-3</v>
+      </c>
+      <c r="J25" s="58">
+        <f t="shared" si="30"/>
+        <v>-9.9022602321320319E-3</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="67">
+        <f>C16-MAX(C16:C18)</f>
+        <v>0</v>
+      </c>
+      <c r="O25" s="67">
+        <f t="shared" ref="O25:U25" si="33">D16-MAX(D16:D18)</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="67">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="67">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="R25" s="67">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="S25" s="67">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="T25" s="67">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="U25" s="69">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7"/>
+      <c r="B26" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="57">
+        <f t="shared" si="30"/>
+        <v>-1.3805742211361993E-2</v>
+      </c>
+      <c r="D26" s="57">
+        <f t="shared" si="30"/>
+        <v>-0.27908368967623703</v>
+      </c>
+      <c r="E26" s="57">
+        <f t="shared" si="30"/>
+        <v>-0.26185705558949296</v>
+      </c>
+      <c r="F26" s="57">
+        <f t="shared" si="30"/>
+        <v>-0.28189981673793496</v>
+      </c>
+      <c r="G26" s="57">
+        <f t="shared" si="30"/>
+        <v>-0.25574832009773996</v>
+      </c>
+      <c r="H26" s="57">
+        <f t="shared" si="30"/>
+        <v>-0.25646915088576699</v>
+      </c>
+      <c r="I26" s="57">
+        <f t="shared" si="30"/>
+        <v>-0.23636530238240705</v>
+      </c>
+      <c r="J26" s="58">
+        <f t="shared" si="30"/>
+        <v>-0.29304215027489305</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="M26" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="N26" s="67">
+        <f>C17-MAX(C16:C18)</f>
+        <v>-0.20463653023824002</v>
+      </c>
+      <c r="O26" s="67">
+        <f t="shared" ref="O26:U26" si="34">D17-MAX(D16:D18)</f>
+        <v>-0.22734880879657898</v>
+      </c>
+      <c r="P26" s="67">
+        <f t="shared" si="34"/>
+        <v>-0.21935858277336601</v>
+      </c>
+      <c r="Q26" s="67">
+        <f t="shared" si="34"/>
+        <v>-0.3976298106292</v>
+      </c>
+      <c r="R26" s="67">
+        <f t="shared" si="34"/>
+        <v>-0.41846670739156999</v>
+      </c>
+      <c r="S26" s="67">
+        <f t="shared" si="34"/>
+        <v>-0.398802687843616</v>
+      </c>
+      <c r="T26" s="67">
+        <f t="shared" si="34"/>
+        <v>-0.42182651191203502</v>
+      </c>
+      <c r="U26" s="69">
+        <f t="shared" si="34"/>
+        <v>-0.41368356750152696</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="8"/>
+      <c r="B27" s="56" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="59">
+        <f t="shared" si="30"/>
+        <v>-1.9511301160659023E-2</v>
+      </c>
+      <c r="D27" s="59">
+        <f t="shared" si="30"/>
+        <v>-0.12427000610873495</v>
+      </c>
+      <c r="E27" s="59">
+        <f t="shared" si="30"/>
+        <v>-9.0647525962125997E-2</v>
+      </c>
+      <c r="F27" s="59">
+        <f t="shared" si="30"/>
+        <v>-0.15802076970067203</v>
+      </c>
+      <c r="G27" s="59">
+        <f t="shared" si="30"/>
+        <v>-0.10361026267562601</v>
+      </c>
+      <c r="H27" s="59">
+        <f t="shared" si="30"/>
+        <v>-7.7855833842395028E-2</v>
+      </c>
+      <c r="I27" s="59">
+        <f t="shared" si="30"/>
+        <v>-0.10920586438607194</v>
+      </c>
+      <c r="J27" s="60">
+        <f t="shared" si="30"/>
+        <v>-9.7116676847893046E-2</v>
+      </c>
+      <c r="L27" s="8"/>
+      <c r="M27" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N27" s="68">
+        <f>C18-MAX(C16:C18)</f>
+        <v>-3.7403787416004031E-2</v>
+      </c>
+      <c r="O27" s="68">
+        <f t="shared" ref="O27:U27" si="35">D18-MAX(D16:D18)</f>
+        <v>-6.6426389737323954E-2</v>
+      </c>
+      <c r="P27" s="68">
+        <f t="shared" si="35"/>
+        <v>-3.8619425778864014E-2</v>
+      </c>
+      <c r="Q27" s="68">
+        <f t="shared" si="35"/>
+        <v>-0.25884544899205897</v>
+      </c>
+      <c r="R27" s="68">
+        <f t="shared" si="35"/>
+        <v>-0.25258399511301199</v>
+      </c>
+      <c r="S27" s="68">
+        <f t="shared" si="35"/>
+        <v>-0.23759926695174105</v>
+      </c>
+      <c r="T27" s="68">
+        <f t="shared" si="35"/>
+        <v>-0.26167990226023297</v>
+      </c>
+      <c r="U27" s="70">
+        <f t="shared" si="35"/>
+        <v>-0.25306658521685998</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="L2:U2"/>
+    <mergeCell ref="L11:U11"/>
+    <mergeCell ref="L20:U20"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2300,28 +3620,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2353,7 +3673,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -2385,7 +3705,7 @@
         <v>0.76939523518631703</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -2415,7 +3735,7 @@
         <v>0.89279169211973097</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -2445,7 +3765,7 @@
         <v>0.77092241905925496</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -2477,7 +3797,7 @@
         <v>0.902565668906536</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -2507,7 +3827,7 @@
         <v>0.77367135003054399</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -2537,22 +3857,22 @@
         <v>0.73610262675626104</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -2584,7 +3904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -2616,7 +3936,7 @@
         <v>0.76847892486255298</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -2646,7 +3966,7 @@
         <v>0.90073304825901002</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -2676,7 +3996,7 @@
         <v>0.76725717776420299</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -2708,7 +4028,7 @@
         <v>0.89431887599267001</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -2738,7 +4058,7 @@
         <v>0.45143555284056203</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -2785,28 +4105,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2838,7 +4158,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -2870,7 +4190,7 @@
         <v>4.5467352872792799E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -2900,7 +4220,7 @@
         <v>2.2658294615613101E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -2930,7 +4250,7 @@
         <v>2.1134223772190298E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -2962,7 +4282,7 @@
         <v>8.1095237199332801E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -2992,7 +4312,7 @@
         <v>1.55801366314775E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -3022,22 +4342,22 @@
         <v>3.2540191616133599E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -3069,7 +4389,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -3101,7 +4421,7 @@
         <v>2.53066193059907E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -3131,7 +4451,7 @@
         <v>1.11770301202718E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -3161,7 +4481,7 @@
         <v>2.55439955871203E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -3193,7 +4513,7 @@
         <v>1.28941685114232E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -3223,7 +4543,7 @@
         <v>0.107761605116556</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -3270,28 +4590,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3323,7 +4643,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -3355,7 +4675,7 @@
         <v>0.801371655696824</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -3385,7 +4705,7 @@
         <v>0.89981756994577899</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -3415,7 +4735,7 @@
         <v>0.81676732040903899</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3447,7 +4767,7 @@
         <v>0.90003669290036303</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -3477,7 +4797,7 @@
         <v>0.79590595556451005</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -3507,22 +4827,22 @@
         <v>0.75978875949921898</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -3554,7 +4874,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -3586,7 +4906,7 @@
         <v>0.80646456764670704</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -3616,7 +4936,7 @@
         <v>0.91265651246527502</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -3646,7 +4966,7 @@
         <v>0.81096867184790999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -3678,7 +4998,7 @@
         <v>0.89401835968861698</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -3708,7 +5028,7 @@
         <v>0.63209081051643401</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>
@@ -3751,32 +5071,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B47BB03-5D51-4927-8C90-D8C37E699AAE}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -3808,7 +5128,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
@@ -3840,7 +5160,7 @@
         <v>0.732305619140738</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="11" t="s">
         <v>17</v>
@@ -3870,7 +5190,7 @@
         <v>0.87981147849189001</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11" t="s">
         <v>18</v>
@@ -3900,7 +5220,7 @@
         <v>0.73198142070461802</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
@@ -3932,7 +5252,7 @@
         <v>0.87069413463699696</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="11" t="s">
         <v>17</v>
@@ -3962,7 +5282,7 @@
         <v>0.70293017668107205</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="12" t="s">
         <v>18</v>
@@ -3992,22 +5312,22 @@
         <v>0.67911932441060296</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="42" t="s">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="45"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
@@ -4039,7 +5359,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
         <v>1</v>
       </c>
@@ -4071,7 +5391,7 @@
         <v>0.72251194197817503</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="11" t="s">
         <v>17</v>
@@ -4101,7 +5421,7 @@
         <v>0.89177021854093497</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="11" t="s">
         <v>18</v>
@@ -4131,7 +5451,7 @@
         <v>0.72950328658821295</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
         <v>2</v>
       </c>
@@ -4163,7 +5483,7 @@
         <v>0.87626812031463097</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="11" t="s">
         <v>17</v>
@@ -4193,7 +5513,7 @@
         <v>0.61867495977612297</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="12" t="s">
         <v>18</v>

</xml_diff>